<commit_message>
chore: add last changes
</commit_message>
<xml_diff>
--- a/src/docs/staticDocs/collection_management_excel.xlsx
+++ b/src/docs/staticDocs/collection_management_excel.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Bibliotecas\Descargas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FANNY BELTRAN\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6989443E-A810-4402-84FB-31C5E942FADD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GESTIONES" sheetId="1" r:id="rId1"/>
@@ -22,29 +23,17 @@
     <definedName name="CODACCION">DETALLE!$A$2:$A$35</definedName>
     <definedName name="TIPOGESTION">DETALLE!$C$2:$C$4</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Renzo Herrera</author>
   </authors>
   <commentList>
-    <comment ref="D1" authorId="0" shapeId="0">
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -78,7 +67,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="0" shapeId="0">
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -428,19 +417,19 @@
     <t xml:space="preserve">Probable Pago </t>
   </si>
   <si>
-    <t>10019100000007253246</t>
+    <t xml:space="preserve">10030500000005364296          </t>
   </si>
   <si>
-    <t>MONDRAGON CHAVEZ ZONIA VICTORIA</t>
+    <t>MINOPE FLORES HECTOR HERNAN</t>
   </si>
   <si>
-    <t xml:space="preserve">cliente renuente infroma que su deuda lo vea con su abogado </t>
+    <t xml:space="preserve">cliente espera remate de la propieda no puede vender por el embargoque posee </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
@@ -598,7 +587,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -634,6 +623,34 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -656,7 +673,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -702,7 +719,7 @@
     <xf numFmtId="0" fontId="10" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="165" fontId="10" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -722,7 +739,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="21" fontId="11" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
@@ -730,23 +750,23 @@
   <cellStyles count="19">
     <cellStyle name="Millares" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="2"/>
-    <cellStyle name="Normal 2 2" xfId="4"/>
-    <cellStyle name="Normal 2 2 2" xfId="6"/>
-    <cellStyle name="Normal 2 2 2 2" xfId="10"/>
-    <cellStyle name="Normal 2 2 2 2 2" xfId="18"/>
-    <cellStyle name="Normal 2 2 2 3" xfId="14"/>
-    <cellStyle name="Normal 2 2 3" xfId="8"/>
-    <cellStyle name="Normal 2 2 3 2" xfId="16"/>
-    <cellStyle name="Normal 2 2 4" xfId="12"/>
-    <cellStyle name="Normal 2 3" xfId="5"/>
-    <cellStyle name="Normal 2 3 2" xfId="9"/>
-    <cellStyle name="Normal 2 3 2 2" xfId="17"/>
-    <cellStyle name="Normal 2 3 3" xfId="13"/>
-    <cellStyle name="Normal 2 4" xfId="7"/>
-    <cellStyle name="Normal 2 4 2" xfId="15"/>
-    <cellStyle name="Normal 2 5" xfId="11"/>
-    <cellStyle name="Normal 4" xfId="3"/>
+    <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Normal 2 2" xfId="4" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Normal 2 2 2" xfId="6" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="Normal 2 2 2 2" xfId="10" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="Normal 2 2 2 2 2" xfId="18" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="Normal 2 2 2 3" xfId="14" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="Normal 2 2 3" xfId="8" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
+    <cellStyle name="Normal 2 2 3 2" xfId="16" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
+    <cellStyle name="Normal 2 2 4" xfId="12" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
+    <cellStyle name="Normal 2 3" xfId="5" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
+    <cellStyle name="Normal 2 3 2" xfId="9" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
+    <cellStyle name="Normal 2 3 2 2" xfId="17" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
+    <cellStyle name="Normal 2 3 3" xfId="13" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
+    <cellStyle name="Normal 2 4" xfId="7" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
+    <cellStyle name="Normal 2 4 2" xfId="15" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
+    <cellStyle name="Normal 2 5" xfId="11" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
+    <cellStyle name="Normal 4" xfId="3" xr:uid="{00000000-0005-0000-0000-000012000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -844,6 +864,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -879,6 +916,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1054,11 +1108,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V6197"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="12.75" customHeight="1"/>
@@ -1161,8 +1215,8 @@
       <c r="A2" s="23" t="s">
         <v>103</v>
       </c>
-      <c r="B2" s="23">
-        <v>116668237</v>
+      <c r="B2" s="34">
+        <v>144371680</v>
       </c>
       <c r="C2" s="33" t="s">
         <v>104</v>
@@ -1170,8 +1224,8 @@
       <c r="D2" s="14">
         <v>45068</v>
       </c>
-      <c r="E2" s="34">
-        <v>0.34652777777777777</v>
+      <c r="E2" s="35">
+        <v>0.46527777777777773</v>
       </c>
       <c r="F2" s="11" t="s">
         <v>49</v>
@@ -19797,9 +19851,9 @@
       <c r="C6197" s="32"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:V2"/>
+  <autoFilter ref="A1:V2" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>TIPOGESTION</formula1>
     </dataValidation>
   </dataValidations>
@@ -19810,7 +19864,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000002000000}">
           <x14:formula1>
             <xm:f>DETALLE!$A$2:$A$38</xm:f>
           </x14:formula1>
@@ -19823,7 +19877,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -20154,7 +20208,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C35"/>
+  <autoFilter ref="A1:C35" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>